<commit_message>
csv working and changes to the parquet exports
</commit_message>
<xml_diff>
--- a/moodys_datahub/data/data_dict.xlsx
+++ b/moodys_datahub/data/data_dict.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/kgp_lib_cbs_dk/Documents/Desktop/moody-s_datahub/moodys_datahub/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgp.lib\OneDrive - CBS - Copenhagen Business School\Desktop\moody-s_datahub\moodys_datahub\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="11_54ED35805B10D55C2BDB2311595ED87656D8DC08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{817AC87B-7219-45D9-B563-72EE48827081}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD8FFE2-977B-4D40-9991-3401343FE025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15060,13 +15060,13 @@
   <dimension ref="A1:E4172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2147" sqref="C2147:C2194"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63.42578125" customWidth="1"/>
-    <col min="3" max="3" width="112" customWidth="1"/>
+    <col min="3" max="3" width="135" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
added "probability of default"
</commit_message>
<xml_diff>
--- a/moodys_datahub/data/data_dict.xlsx
+++ b/moodys_datahub/data/data_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgp.lib\OneDrive - CBS - Copenhagen Business School\Desktop\moody-s_datahub\moodys_datahub\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/kgp_lib_cbs_dk/Documents/Desktop/moody-s_datahub/moodys_datahub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD8FFE2-977B-4D40-9991-3401343FE025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{1AD8FFE2-977B-4D40-9991-3401343FE025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3120DC68-F5A7-46E1-9398-F02B53EC89BE}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16688" uniqueCount="4805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16820" uniqueCount="4807">
   <si>
     <t>Data Product</t>
   </si>
@@ -14671,6 +14671,12 @@
   </si>
   <si>
     <t>segment_data</t>
+  </si>
+  <si>
+    <t>Probability of Default</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -15057,10 +15063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4172"/>
+  <dimension ref="A1:E4205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4179" sqref="C4179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85992,6 +85998,567 @@
         <v>332</v>
       </c>
     </row>
+    <row r="4173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4173" s="1">
+        <v>3612</v>
+      </c>
+      <c r="B4173" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4173" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4173" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4173" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4174" s="1">
+        <v>3613</v>
+      </c>
+      <c r="B4174" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4174" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4174" t="s">
+        <v>2062</v>
+      </c>
+      <c r="E4174" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4175" s="1">
+        <v>3614</v>
+      </c>
+      <c r="B4175" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4175" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4175" t="s">
+        <v>3913</v>
+      </c>
+      <c r="E4175" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4176" s="1">
+        <v>3615</v>
+      </c>
+      <c r="B4176" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4176" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4176" t="s">
+        <v>3764</v>
+      </c>
+      <c r="E4176" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4177" s="1">
+        <v>3616</v>
+      </c>
+      <c r="B4177" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4177" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4177" t="s">
+        <v>3916</v>
+      </c>
+      <c r="E4177" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4178" s="1">
+        <v>3617</v>
+      </c>
+      <c r="B4178" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4178" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4178" t="s">
+        <v>3918</v>
+      </c>
+      <c r="E4178" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4179" s="1">
+        <v>3618</v>
+      </c>
+      <c r="B4179" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4179" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4179" t="s">
+        <v>3920</v>
+      </c>
+      <c r="E4179" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4180" s="1">
+        <v>3619</v>
+      </c>
+      <c r="B4180" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4180" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4180" t="s">
+        <v>3922</v>
+      </c>
+      <c r="E4180" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4181" s="1">
+        <v>3620</v>
+      </c>
+      <c r="B4181" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4181" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4181" t="s">
+        <v>3924</v>
+      </c>
+      <c r="E4181" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4182" s="1">
+        <v>3621</v>
+      </c>
+      <c r="B4182" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4182" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4182" t="s">
+        <v>3926</v>
+      </c>
+      <c r="E4182" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4183" s="1">
+        <v>3622</v>
+      </c>
+      <c r="B4183" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4183" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4183" t="s">
+        <v>3928</v>
+      </c>
+      <c r="E4183" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4184" s="1">
+        <v>3623</v>
+      </c>
+      <c r="B4184" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4184" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4184" t="s">
+        <v>3930</v>
+      </c>
+      <c r="E4184" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4185" s="1">
+        <v>3624</v>
+      </c>
+      <c r="B4185" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4185" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4185" t="s">
+        <v>3932</v>
+      </c>
+      <c r="E4185" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4186" s="1">
+        <v>3625</v>
+      </c>
+      <c r="B4186" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4186" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4186" t="s">
+        <v>3934</v>
+      </c>
+      <c r="E4186" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4187" s="1">
+        <v>3626</v>
+      </c>
+      <c r="B4187" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4187" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4187" t="s">
+        <v>3936</v>
+      </c>
+      <c r="E4187" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4188" s="1">
+        <v>3627</v>
+      </c>
+      <c r="B4188" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4188" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4188" t="s">
+        <v>3938</v>
+      </c>
+      <c r="E4188" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4189" s="1">
+        <v>3628</v>
+      </c>
+      <c r="B4189" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4189" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4189" t="s">
+        <v>3940</v>
+      </c>
+      <c r="E4189" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4190" s="1">
+        <v>3629</v>
+      </c>
+      <c r="B4190" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4190" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4190" t="s">
+        <v>3942</v>
+      </c>
+      <c r="E4190" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4191" s="1">
+        <v>3630</v>
+      </c>
+      <c r="B4191" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4191" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4191" t="s">
+        <v>3944</v>
+      </c>
+      <c r="E4191" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4192" s="1">
+        <v>3631</v>
+      </c>
+      <c r="B4192" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4192" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4192" t="s">
+        <v>3946</v>
+      </c>
+      <c r="E4192" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4193" s="1">
+        <v>3632</v>
+      </c>
+      <c r="B4193" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4193" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4193" t="s">
+        <v>3948</v>
+      </c>
+      <c r="E4193" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4194" s="1">
+        <v>3633</v>
+      </c>
+      <c r="B4194" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4194" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4194" t="s">
+        <v>3950</v>
+      </c>
+      <c r="E4194" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4195" s="1">
+        <v>3634</v>
+      </c>
+      <c r="B4195" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4195" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4195" t="s">
+        <v>3952</v>
+      </c>
+      <c r="E4195" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4196" s="1">
+        <v>3635</v>
+      </c>
+      <c r="B4196" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4196" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4196" t="s">
+        <v>3954</v>
+      </c>
+      <c r="E4196" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4197" s="1">
+        <v>3636</v>
+      </c>
+      <c r="B4197" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4197" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4197" t="s">
+        <v>3956</v>
+      </c>
+      <c r="E4197" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4198" s="1">
+        <v>3637</v>
+      </c>
+      <c r="B4198" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4198" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4198" t="s">
+        <v>3958</v>
+      </c>
+      <c r="E4198" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4199" s="1">
+        <v>3638</v>
+      </c>
+      <c r="B4199" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4199" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4199" t="s">
+        <v>3960</v>
+      </c>
+      <c r="E4199" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4200" s="1">
+        <v>3639</v>
+      </c>
+      <c r="B4200" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4200" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4200" t="s">
+        <v>3962</v>
+      </c>
+      <c r="E4200" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4201" s="1">
+        <v>3640</v>
+      </c>
+      <c r="B4201" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4201" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4201" t="s">
+        <v>3964</v>
+      </c>
+      <c r="E4201" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4202" s="1">
+        <v>3641</v>
+      </c>
+      <c r="B4202" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4202" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4202" t="s">
+        <v>3966</v>
+      </c>
+      <c r="E4202" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4203" s="1">
+        <v>3642</v>
+      </c>
+      <c r="B4203" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4203" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4203" t="s">
+        <v>3968</v>
+      </c>
+      <c r="E4203" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4204" s="1">
+        <v>3643</v>
+      </c>
+      <c r="B4204" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4204" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4204" t="s">
+        <v>3970</v>
+      </c>
+      <c r="E4204" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4205" s="1">
+        <v>3644</v>
+      </c>
+      <c r="B4205" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C4205" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D4205" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4205" t="s">
+        <v>4806</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E4172" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4172">

</xml_diff>